<commit_message>
Updated TestData and Utilities.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\OLB\InstantOpen_Automation\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\workspace_automation\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE6637E-5A70-496F-AE37-6924FE0E5501}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580EE3AF-FD41-4573-B2C2-73BEDE52B4AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="DNA_Upgrade" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -258,13 +259,49 @@
   </si>
   <si>
     <t>8229319</t>
+  </si>
+  <si>
+    <t>C23835_VerifyInformationAboutAccountandProductSelection</t>
+  </si>
+  <si>
+    <t>InformationHeaderMsg</t>
+  </si>
+  <si>
+    <t>InformationMsgContent</t>
+  </si>
+  <si>
+    <t>Let’s open your new account!</t>
+  </si>
+  <si>
+    <t>CheckingAccountHeader</t>
+  </si>
+  <si>
+    <t>Here are your checking account options:</t>
+  </si>
+  <si>
+    <t>BottomInfoMsg</t>
+  </si>
+  <si>
+    <t>Are you looking for loans, credit cards or other ways to save?</t>
+  </si>
+  <si>
+    <t>As a new Member, you automatically get a Savings account! To get you started, we will deposit $5.00 into your new account. We should also mention there’s no monthly fee.</t>
+  </si>
+  <si>
+    <t>C23836_VerifyCheckingOptionsListedTopOfAccountSelection</t>
+  </si>
+  <si>
+    <t>C24249_VerifyUserNeedsToCheckAccountOptionToProccedNextPage</t>
+  </si>
+  <si>
+    <t>C23901_VerifyCustomizeOptionForUserCheckingAccount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +325,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -310,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -320,6 +363,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -637,14 +681,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -787,17 +831,63 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1162,24 +1252,27 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{CE5681DE-E3B0-4B04-A498-3F0E690ACDEC}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{D17112A8-C091-4245-B00A-7EF7858629A5}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{189F3566-96EB-48EC-A09E-5B29DF50EDC1}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{3F747B60-F7FB-475B-B6A7-094CF3CD5A07}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{09B28CA0-61E7-4E25-A1B4-3F4BBC1FC458}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{C747F255-77AD-4D67-834C-AF76DD58D60A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U5" sqref="U5"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
@@ -1194,9 +1287,13 @@
     <col min="17" max="17" width="12.42578125" customWidth="1"/>
     <col min="19" max="19" width="23.28515625" customWidth="1"/>
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="54.140625" customWidth="1"/>
+    <col min="26" max="26" width="41" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="64.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1266,8 +1363,20 @@
       <c r="W1" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1450,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>48</v>
       </c>
@@ -1358,7 +1467,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1381,7 +1490,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
@@ -1398,39 +1507,87 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1496,6 +1653,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added and modified scripts
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\workspace_automation\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580EE3AF-FD41-4573-B2C2-73BEDE52B4AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A941635-41C7-41DC-A8C3-470FD888499B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="DNA_Upgrade" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -295,6 +294,27 @@
   </si>
   <si>
     <t>C23901_VerifyCustomizeOptionForUserCheckingAccount</t>
+  </si>
+  <si>
+    <t>C24253_VerifyMoreInfoAboutOptionsOfCheckingAccount</t>
+  </si>
+  <si>
+    <t>C24255_VerifyChangeAbilityOfCustomizeOption</t>
+  </si>
+  <si>
+    <t>C23717_VerifyUserIsAbleToViewOtherProducts</t>
+  </si>
+  <si>
+    <t>C23720_VerifyCreditCardDetails</t>
+  </si>
+  <si>
+    <t>C23721_VerifyVehicleLoansAndRefinanceOptions</t>
+  </si>
+  <si>
+    <t>C24279_VerifyAdditionalProductsAreSeparatedIntoAdditionalAccordions</t>
+  </si>
+  <si>
+    <t>C24287_VerifyCertainServiceOptionsSelected</t>
   </si>
 </sst>
 </file>
@@ -682,12 +702,12 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -890,83 +910,160 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="F32" s="1"/>
     </row>
@@ -1255,9 +1352,16 @@
     <hyperlink ref="B10" r:id="rId8" xr:uid="{3F747B60-F7FB-475B-B6A7-094CF3CD5A07}"/>
     <hyperlink ref="B11" r:id="rId9" xr:uid="{09B28CA0-61E7-4E25-A1B4-3F4BBC1FC458}"/>
     <hyperlink ref="B12" r:id="rId10" xr:uid="{C747F255-77AD-4D67-834C-AF76DD58D60A}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{F3DC7F88-7E83-4629-9007-E58FC25F8D69}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{9EDB57B1-1B4D-4543-9D2B-DB6409AC8124}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{A76D10E6-FB61-4DB0-B530-92F38B132BEF}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{6578A5F1-046C-42B7-B012-4F99E74D1481}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{94E95772-BACB-458D-BB30-A8A162C8AE13}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{36479EDA-49A9-47AA-8717-A62FE8A23B3A}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{D2172A3E-46DB-4E52-B9EC-E32082573A44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -1266,13 +1370,13 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
@@ -1576,77 +1680,174 @@
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
+      <c r="X11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
+      <c r="X12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
       <c r="B13" s="2"/>
+      <c r="X13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z13" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="X16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="X17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z17" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA17" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>

</xml_diff>

<commit_message>
New scripts added for SelectAccounts
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\workspace_automation\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A941635-41C7-41DC-A8C3-470FD888499B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE950CA-CAED-49B9-8DD7-735CE1968169}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="111">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -315,6 +315,51 @@
   </si>
   <si>
     <t>C24287_VerifyCertainServiceOptionsSelected</t>
+  </si>
+  <si>
+    <t>C24250_VerifyAdditionalOptionsToApplicants</t>
+  </si>
+  <si>
+    <t>C23722_VerifypersonalLoanOptionAndSelect</t>
+  </si>
+  <si>
+    <t>C24252_VerifyEdocumentAddedAsAdditionalSeviceOption</t>
+  </si>
+  <si>
+    <t>C24289_VerifyMoreDetailsAboutEdocument</t>
+  </si>
+  <si>
+    <t>C23736_VerifyUserIsAbleToGoBackToTheHomePageOrAdvanceToNextPage</t>
+  </si>
+  <si>
+    <t>C23724_WizardToSelectRightCertificateOfDeposit</t>
+  </si>
+  <si>
+    <t>LoanAmount</t>
+  </si>
+  <si>
+    <t>LoanTerm</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>01/08/1986</t>
+  </si>
+  <si>
+    <t>C23719_WizardToSelectRightMoneyMarket</t>
+  </si>
+  <si>
+    <t>C23718_AdditonalSavingAccount</t>
+  </si>
+  <si>
+    <t>987567911</t>
+  </si>
+  <si>
+    <t>987567912</t>
+  </si>
+  <si>
+    <t>987567913</t>
   </si>
 </sst>
 </file>
@@ -373,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -384,6 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -701,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,35 +1062,123 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1359,19 +1493,27 @@
     <hyperlink ref="B17" r:id="rId15" xr:uid="{94E95772-BACB-458D-BB30-A8A162C8AE13}"/>
     <hyperlink ref="B18" r:id="rId16" xr:uid="{36479EDA-49A9-47AA-8717-A62FE8A23B3A}"/>
     <hyperlink ref="B19" r:id="rId17" xr:uid="{D2172A3E-46DB-4E52-B9EC-E32082573A44}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{12BC60C7-8659-4072-A664-3741245A5F12}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{635F0E1D-B478-4E51-9A7D-2B7D9F1B173A}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{A74BCB79-A71E-4F9A-8336-66BD4488C1FA}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{5174849B-42DD-4DC7-8B20-88A3E1422071}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{F05B886E-65D4-493F-95E4-CF8AB9853339}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{E0D67863-0392-4AD7-842B-6A52C2F35A45}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{98BB69DA-E313-4AAB-B96F-19B04FF87635}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{73026259-7FDE-4F98-889D-27C133635FE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,9 +1537,11 @@
     <col min="25" max="25" width="54.140625" customWidth="1"/>
     <col min="26" max="26" width="41" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1479,8 +1623,14 @@
       <c r="AA1" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1537,7 +1687,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1554,7 +1704,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>48</v>
       </c>
@@ -1571,7 +1721,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1594,7 +1744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
@@ -1611,7 +1761,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -1631,7 +1781,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
@@ -1651,7 +1801,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1659,7 +1809,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -1679,7 +1829,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1699,7 +1849,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -1718,7 +1868,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -1733,7 +1883,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>92</v>
       </c>
@@ -1747,7 +1897,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -1761,7 +1911,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1778,7 +1928,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1798,56 +1948,348 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="X18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z18" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z19" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y20" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z21" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+      <c r="X22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="D23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC23" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="D24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="8"/>
+      <c r="AD25" s="6"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>

</xml_diff>

<commit_message>
02/12: New Scripts commited.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\workspace_automation\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE950CA-CAED-49B9-8DD7-735CE1968169}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="DNA_Upgrade" sheetId="3" r:id="rId3"/>
+    <sheet name="ProdData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="316">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -360,12 +355,627 @@
   </si>
   <si>
     <t>987567913</t>
+  </si>
+  <si>
+    <t>C23881_VerifyVehicleLoanInfo</t>
+  </si>
+  <si>
+    <t>ProdTitle1</t>
+  </si>
+  <si>
+    <t>ProdTitle2</t>
+  </si>
+  <si>
+    <t>ProdTitle3</t>
+  </si>
+  <si>
+    <t>ProdTitle4</t>
+  </si>
+  <si>
+    <t>ProdTitle5</t>
+  </si>
+  <si>
+    <t>ProdInfo1</t>
+  </si>
+  <si>
+    <t>ProdInfo2</t>
+  </si>
+  <si>
+    <t>ProdInfo3</t>
+  </si>
+  <si>
+    <t>ProdInfo4</t>
+  </si>
+  <si>
+    <t>ProdInfo5</t>
+  </si>
+  <si>
+    <t>ProdMin1</t>
+  </si>
+  <si>
+    <t>ProdMin2</t>
+  </si>
+  <si>
+    <t>ProdMin3</t>
+  </si>
+  <si>
+    <t>ProdMin4</t>
+  </si>
+  <si>
+    <t>ProdMin5</t>
+  </si>
+  <si>
+    <t>ProdDesc1</t>
+  </si>
+  <si>
+    <t>ProdDesc2</t>
+  </si>
+  <si>
+    <t>ProdDesc3</t>
+  </si>
+  <si>
+    <t>ProdDesc4</t>
+  </si>
+  <si>
+    <t>ProdDesc5</t>
+  </si>
+  <si>
+    <t>ProdDesc6</t>
+  </si>
+  <si>
+    <t>ProdDesc7</t>
+  </si>
+  <si>
+    <t>ProdText1</t>
+  </si>
+  <si>
+    <t>ProdText2</t>
+  </si>
+  <si>
+    <t>ProdText3</t>
+  </si>
+  <si>
+    <t>ProdText4</t>
+  </si>
+  <si>
+    <t>OtherTxt1</t>
+  </si>
+  <si>
+    <t>OtherTxt2</t>
+  </si>
+  <si>
+    <t>OtherTxt3</t>
+  </si>
+  <si>
+    <t>OtherTxt4</t>
+  </si>
+  <si>
+    <t>OtherTxt5</t>
+  </si>
+  <si>
+    <t>OtherTxt6</t>
+  </si>
+  <si>
+    <t>OtherTxt7</t>
+  </si>
+  <si>
+    <t>OtherTxt8</t>
+  </si>
+  <si>
+    <t>OtherTxt9</t>
+  </si>
+  <si>
+    <t>Auto Loan (New or Used)</t>
+  </si>
+  <si>
+    <t>Boat Loans (New or Used)</t>
+  </si>
+  <si>
+    <t>RV/Camper Loans (New or Used)</t>
+  </si>
+  <si>
+    <t>Personal Watercraft (New or Used)</t>
+  </si>
+  <si>
+    <t>Motorcycle Loans (New or Used)</t>
+  </si>
+  <si>
+    <t>Refinance your Auto Loan with TDECU</t>
+  </si>
+  <si>
+    <t>Refinance your Motorcycle Loan with TDECU</t>
+  </si>
+  <si>
+    <t>Refinance your RV/Camper Loan with TDECU</t>
+  </si>
+  <si>
+    <t>Refinance your Boat Loan with TDECU</t>
+  </si>
+  <si>
+    <t>ATV/UTV Loans (New or Used)</t>
+  </si>
+  <si>
+    <t>$10,550.00</t>
+  </si>
+  <si>
+    <t>$21,568.00</t>
+  </si>
+  <si>
+    <t>*Which type of Vehicle Loan are you requesting?</t>
+  </si>
+  <si>
+    <t>*What loan amount are you requesting?</t>
+  </si>
+  <si>
+    <t>*What was the Purchase Price of the vehicle?</t>
+  </si>
+  <si>
+    <t>Make:</t>
+  </si>
+  <si>
+    <t>Model:</t>
+  </si>
+  <si>
+    <t>Year:</t>
+  </si>
+  <si>
+    <t>Mileage:</t>
+  </si>
+  <si>
+    <t>What is the Vehicle Identification Number (VIN)?</t>
+  </si>
+  <si>
+    <t>Please provide information for the vehicle loan that you are requesting below:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Back </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Continue </t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $100,000</t>
+  </si>
+  <si>
+    <t>Harley Davidson</t>
+  </si>
+  <si>
+    <t>Fat Boy</t>
+  </si>
+  <si>
+    <t>7256</t>
+  </si>
+  <si>
+    <t>6546df54sdfwef41</t>
+  </si>
+  <si>
+    <t>C23884_VerifyVehicleLoanReqFields</t>
+  </si>
+  <si>
+    <t>Please select a product type.</t>
+  </si>
+  <si>
+    <t>lksdjf9092kf0d</t>
+  </si>
+  <si>
+    <t>Please select an item from the drop down list.</t>
+  </si>
+  <si>
+    <t>Please enter an Amount.</t>
+  </si>
+  <si>
+    <t>Please enter a vehicle VIN</t>
+  </si>
+  <si>
+    <t>C23885_VerifyValidVehicleInfo</t>
+  </si>
+  <si>
+    <t>$1,000.00</t>
+  </si>
+  <si>
+    <t>letters</t>
+  </si>
+  <si>
+    <t>("$#@]</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>$13,256.22</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Wrangler</t>
+  </si>
+  <si>
+    <t>20125</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>lkjio8sk3lkjfs</t>
+  </si>
+  <si>
+    <t>Please enter a value between $5,000 and $100,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $125,000</t>
+  </si>
+  <si>
+    <t>Must enter a four digit year between 1900 and 2021</t>
+  </si>
+  <si>
+    <t>1899</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>1900</t>
+  </si>
+  <si>
+    <t>Please enter whole numbers only.</t>
+  </si>
+  <si>
+    <t>16872</t>
+  </si>
+  <si>
+    <t>C23882_VerifyVehicleLoanLimit</t>
+  </si>
+  <si>
+    <t>$6,500.00</t>
+  </si>
+  <si>
+    <t>$12,222.00</t>
+  </si>
+  <si>
+    <t>Minimum $5,000.00</t>
+  </si>
+  <si>
+    <t>C23883_VerifyVehicleLoanMinMax</t>
+  </si>
+  <si>
+    <t>$6,789.00</t>
+  </si>
+  <si>
+    <t>Please enter a value between $5,000 and $150,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $150,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $1,000,000</t>
+  </si>
+  <si>
+    <t>C23855_VerifyPersonalLoanInfo</t>
+  </si>
+  <si>
+    <t>My Way Loan: $4,000</t>
+  </si>
+  <si>
+    <t>My Way Loan: $6,000</t>
+  </si>
+  <si>
+    <t>My Way Loan: $7,000</t>
+  </si>
+  <si>
+    <t>Personal Loan</t>
+  </si>
+  <si>
+    <t>Home Advantage Personal Loan</t>
+  </si>
+  <si>
+    <t>Cash $tash&amp;trade; Line of Credit</t>
+  </si>
+  <si>
+    <t>Certificate of Deposit Secured Loan</t>
+  </si>
+  <si>
+    <t>Share Secured Loan</t>
+  </si>
+  <si>
+    <t>$5,000.00</t>
+  </si>
+  <si>
+    <t>Please enter the information about the line of credit loan you are requesting below:</t>
+  </si>
+  <si>
+    <t>*Type of Loan Requested:</t>
+  </si>
+  <si>
+    <t>*Loan Amount Requested:</t>
+  </si>
+  <si>
+    <t>C23856_VerifyPersonalLoanLimit</t>
+  </si>
+  <si>
+    <t>Minimum $1,000.00</t>
+  </si>
+  <si>
+    <t>$13,000.00</t>
+  </si>
+  <si>
+    <t>$25,147.00</t>
+  </si>
+  <si>
+    <t>Please enter a value between $4,000 and $4,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $6,000 and $6,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $7,000 and $7,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $15,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $35,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $1,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $250,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $500 and $250,000</t>
+  </si>
+  <si>
+    <t>C23891_VerifyPersonalLoanMinMax</t>
+  </si>
+  <si>
+    <t>C23893_VerifyValidPersonalLoanInfo</t>
+  </si>
+  <si>
+    <t>C24273_VerifyAdditionalLoanInfo</t>
+  </si>
+  <si>
+    <t>Applicant Information</t>
+  </si>
+  <si>
+    <t>Identification Information</t>
+  </si>
+  <si>
+    <t>Loan Information</t>
+  </si>
+  <si>
+    <t>Please select at least one type of account below.</t>
+  </si>
+  <si>
+    <t>023465789</t>
+  </si>
+  <si>
+    <t>02061980</t>
+  </si>
+  <si>
+    <t>C24274_VerifyHousingTypeField</t>
+  </si>
+  <si>
+    <t>Type of Housing.</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Own</t>
+  </si>
+  <si>
+    <t>Mortgage</t>
+  </si>
+  <si>
+    <t>8229386</t>
+  </si>
+  <si>
+    <t>456127890</t>
+  </si>
+  <si>
+    <t>01011980</t>
+  </si>
+  <si>
+    <t>C24275_VerifyHousingPaymentField</t>
+  </si>
+  <si>
+    <t>1000000000.01</t>
+  </si>
+  <si>
+    <t>$1,252.00</t>
+  </si>
+  <si>
+    <t>Please enter a value between $0 and $1,000,000,000</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>01012010</t>
+  </si>
+  <si>
+    <t>01012025</t>
+  </si>
+  <si>
+    <t>C24278_VerifyMonthlyIncomeField</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Eagle Creek</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>$5,500.00</t>
+  </si>
+  <si>
+    <t>C24280_VerifyLengthofEmploymentFields</t>
+  </si>
+  <si>
+    <t>xy</t>
+  </si>
+  <si>
+    <t>!+</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Please enter a value between 0 and 99</t>
+  </si>
+  <si>
+    <t>Please enter a value between 0 and 12</t>
+  </si>
+  <si>
+    <t>8229312</t>
+  </si>
+  <si>
+    <t>168151171</t>
+  </si>
+  <si>
+    <t>C24276_VerifyLivedAtAddressFields</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>?&amp;</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>C24281_VerifyEmployerField</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cu%re^t Em9l0yer </t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A1Z9</t>
+  </si>
+  <si>
+    <t>02062015</t>
+  </si>
+  <si>
+    <t>02062030</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Current Employer</t>
+  </si>
+  <si>
+    <t>pRE^i0u$ EMP!oy3#</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Please enter how long you have been employed in years and months.</t>
+  </si>
+  <si>
+    <t>67890</t>
+  </si>
+  <si>
+    <t>02062010</t>
+  </si>
+  <si>
+    <t>02062025</t>
+  </si>
+  <si>
+    <t>C24282_VerifyPreviousEmployerField</t>
+  </si>
+  <si>
+    <t>C24283_VerifyPreviousIncomeField</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>(10</t>
+  </si>
+  <si>
+    <t>1000000001</t>
+  </si>
+  <si>
+    <t>prevIncome</t>
+  </si>
+  <si>
+    <t>$3,333.33</t>
+  </si>
+  <si>
+    <t>03132016</t>
+  </si>
+  <si>
+    <t>02272026</t>
+  </si>
+  <si>
+    <t>C24284_VerifyLengthofPrevEmpFields</t>
+  </si>
+  <si>
+    <t>Yr</t>
+  </si>
+  <si>
+    <t>*&lt;</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>C24277_VerifyEmpStatusField</t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>Part Time</t>
+  </si>
+  <si>
+    <t>Please Select an Item from the drop down list.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,7 +1028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -430,6 +1040,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,7 +1104,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -543,7 +1156,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -737,18 +1350,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:D27"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,86 +1795,306 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
+      <c r="A29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
+      <c r="A30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
+      <c r="A31" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
+      <c r="A32" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>244</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>252</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>259</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>266</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>276</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>282</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>298</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>299</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>312</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="F48" s="1"/>
     </row>
@@ -1476,42 +2309,62 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{58421974-CE0C-4F41-840C-D502238A7A0E}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{9200CF74-EA66-4F97-9C5C-20C8F9562672}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{3C3037BD-5204-4A9A-ABE3-C497536C366E}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{8D06D0BD-DDF7-4C4B-AF1A-8E8739C0DA4A}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{CE5681DE-E3B0-4B04-A498-3F0E690ACDEC}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{D17112A8-C091-4245-B00A-7EF7858629A5}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{189F3566-96EB-48EC-A09E-5B29DF50EDC1}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{3F747B60-F7FB-475B-B6A7-094CF3CD5A07}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{09B28CA0-61E7-4E25-A1B4-3F4BBC1FC458}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{C747F255-77AD-4D67-834C-AF76DD58D60A}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{F3DC7F88-7E83-4629-9007-E58FC25F8D69}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{9EDB57B1-1B4D-4543-9D2B-DB6409AC8124}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{A76D10E6-FB61-4DB0-B530-92F38B132BEF}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{6578A5F1-046C-42B7-B012-4F99E74D1481}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{94E95772-BACB-458D-BB30-A8A162C8AE13}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{36479EDA-49A9-47AA-8717-A62FE8A23B3A}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{D2172A3E-46DB-4E52-B9EC-E32082573A44}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{12BC60C7-8659-4072-A664-3741245A5F12}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{635F0E1D-B478-4E51-9A7D-2B7D9F1B173A}"/>
-    <hyperlink ref="B22" r:id="rId20" xr:uid="{A74BCB79-A71E-4F9A-8336-66BD4488C1FA}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{5174849B-42DD-4DC7-8B20-88A3E1422071}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{F05B886E-65D4-493F-95E4-CF8AB9853339}"/>
-    <hyperlink ref="B25" r:id="rId23" xr:uid="{E0D67863-0392-4AD7-842B-6A52C2F35A45}"/>
-    <hyperlink ref="B26" r:id="rId24" xr:uid="{98BB69DA-E313-4AAB-B96F-19B04FF87635}"/>
-    <hyperlink ref="B27" r:id="rId25" xr:uid="{73026259-7FDE-4F98-889D-27C133635FE0}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B20" r:id="rId18"/>
+    <hyperlink ref="B21" r:id="rId19"/>
+    <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B23" r:id="rId21"/>
+    <hyperlink ref="B24" r:id="rId22"/>
+    <hyperlink ref="B25" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
+    <hyperlink ref="B27" r:id="rId25"/>
+    <hyperlink ref="B28" r:id="rId26"/>
+    <hyperlink ref="B29" r:id="rId27"/>
+    <hyperlink ref="B30" r:id="rId28"/>
+    <hyperlink ref="B31" r:id="rId29"/>
+    <hyperlink ref="B32" r:id="rId30"/>
+    <hyperlink ref="B33" r:id="rId31"/>
+    <hyperlink ref="B34" r:id="rId32"/>
+    <hyperlink ref="B35" r:id="rId33"/>
+    <hyperlink ref="B36" r:id="rId34"/>
+    <hyperlink ref="B37" r:id="rId35"/>
+    <hyperlink ref="B38" r:id="rId36"/>
+    <hyperlink ref="B39" r:id="rId37"/>
+    <hyperlink ref="B40" r:id="rId38"/>
+    <hyperlink ref="B41" r:id="rId39"/>
+    <hyperlink ref="B42" r:id="rId40"/>
+    <hyperlink ref="B43" r:id="rId41"/>
+    <hyperlink ref="B44" r:id="rId42"/>
+    <hyperlink ref="B45" r:id="rId43"/>
+    <hyperlink ref="B46" r:id="rId44"/>
+    <hyperlink ref="B47" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
@@ -2301,7 +3154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A8A316-7525-4895-A0B5-7D3B92BB01F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2376,4 +3229,1112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L2" s="6">
+        <v>5</v>
+      </c>
+      <c r="M2" s="6">
+        <v>10550</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="O2" s="6">
+        <v>21568</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>2017</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="6">
+        <v>5000</v>
+      </c>
+      <c r="H3" s="6">
+        <v>10000</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2000</v>
+      </c>
+      <c r="H4" s="6">
+        <v>130000.55</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1000</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="N4" s="6">
+        <v>13256.22</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="AG4" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>16872.560000000001</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="6">
+        <v>6500</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I5" s="6">
+        <v>12222</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K5" s="6">
+        <v>7</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="6">
+        <v>999.99</v>
+      </c>
+      <c r="H6" s="6">
+        <v>100001.01</v>
+      </c>
+      <c r="I6" s="6">
+        <v>125000.01</v>
+      </c>
+      <c r="J6" s="6">
+        <v>4999.99</v>
+      </c>
+      <c r="K6" s="6">
+        <v>150000.01</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1000000.99</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6789</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="L7" s="6">
+        <v>5000</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="M8" s="6">
+        <v>13000</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="L9" s="6">
+        <v>5</v>
+      </c>
+      <c r="M9" s="6">
+        <v>25147</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE9" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="AG9" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AH9" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G10" s="6">
+        <v>800</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1000.11</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G11" s="6">
+        <v>3000</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC11" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD11" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G12" s="6">
+        <v>4000</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB12" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC12" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD12" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G13" s="6">
+        <v>6000</v>
+      </c>
+      <c r="H13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1252</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD13" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF13" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG13" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH13" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="G14" s="6">
+        <v>35000</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2222</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="U14" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="V14" s="6">
+        <v>5500</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB14" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC14" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD14" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AE14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF14" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG14" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH14" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="6">
+        <v>100</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC15" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD15" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="G16" s="6">
+        <v>7000</v>
+      </c>
+      <c r="H16" s="6">
+        <v>101</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y16" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB16" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC16" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD16" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+    </row>
+    <row r="17" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G17" s="6">
+        <v>250000</v>
+      </c>
+      <c r="H17" s="6">
+        <v>4000</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB17" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC17" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD17" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF17" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG17" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="AH17" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" s="6">
+        <v>500</v>
+      </c>
+      <c r="H18" s="6">
+        <v>452.67</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="R18" s="6">
+        <v>7000</v>
+      </c>
+      <c r="S18" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="U18" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="X18" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC18" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD18" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF18" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="AG18" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="AH18" s="9" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G19" s="6">
+        <v>5000</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1954.23</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="K19" s="6">
+        <v>4444.4399999999996</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="S19" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="V19" s="6">
+        <v>3333.33</v>
+      </c>
+      <c r="W19" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="X19" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y19" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB19" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC19" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD19" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF19" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG19" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="AH19" s="9" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="G20" s="6">
+        <v>123456.78</v>
+      </c>
+      <c r="H20" s="6">
+        <v>200</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="X20" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB20" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC20" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD20" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="G21" s="6">
+        <v>15000</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC21" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD21" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
02/12: Latest changes of InstantOpen.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA0FE4E-B752-4E06-A022-A9F3F661D30C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="324">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -970,12 +976,38 @@
   </si>
   <si>
     <t>Please Select an Item from the drop down list.</t>
+  </si>
+  <si>
+    <t>C23843_NonMemberCreditCardtLimit</t>
+  </si>
+  <si>
+    <t>C23889_NonMemberUserNeedToKnowMaxAndMinCreditLimit</t>
+  </si>
+  <si>
+    <t>C23890_NonMemberUserMustEnterTypeAndLimit</t>
+  </si>
+  <si>
+    <t>C23838_NonMemberChangeSelectedCreditCardOption</t>
+  </si>
+  <si>
+    <t>C23761_NonMemberUserToKnowAboutPersonalInfo</t>
+  </si>
+  <si>
+    <t>C23762_NonMemberUserReceivesPopupForInvalidCharecters</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    By selecting Continue below you agree to not use any TDECU accounts, services or products for unlawful or illegal gambling practices in accordance with the Unlawful Internet Gambling Enforcement Act (UIGEA).
+    </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1028,7 +1060,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1043,6 +1075,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1350,18 +1385,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,71 +2129,137 @@
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
+    <row r="48" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
+    <row r="49" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
+    <row r="50" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="4"/>
+    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
+    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+    <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="F64" s="1"/>
     </row>
@@ -2309,64 +2410,70 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
-    <hyperlink ref="B23" r:id="rId21"/>
-    <hyperlink ref="B24" r:id="rId22"/>
-    <hyperlink ref="B25" r:id="rId23"/>
-    <hyperlink ref="B26" r:id="rId24"/>
-    <hyperlink ref="B27" r:id="rId25"/>
-    <hyperlink ref="B28" r:id="rId26"/>
-    <hyperlink ref="B29" r:id="rId27"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B31" r:id="rId29"/>
-    <hyperlink ref="B32" r:id="rId30"/>
-    <hyperlink ref="B33" r:id="rId31"/>
-    <hyperlink ref="B34" r:id="rId32"/>
-    <hyperlink ref="B35" r:id="rId33"/>
-    <hyperlink ref="B36" r:id="rId34"/>
-    <hyperlink ref="B37" r:id="rId35"/>
-    <hyperlink ref="B38" r:id="rId36"/>
-    <hyperlink ref="B39" r:id="rId37"/>
-    <hyperlink ref="B40" r:id="rId38"/>
-    <hyperlink ref="B41" r:id="rId39"/>
-    <hyperlink ref="B42" r:id="rId40"/>
-    <hyperlink ref="B43" r:id="rId41"/>
-    <hyperlink ref="B44" r:id="rId42"/>
-    <hyperlink ref="B45" r:id="rId43"/>
-    <hyperlink ref="B46" r:id="rId44"/>
-    <hyperlink ref="B47" r:id="rId45"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{18250720-CBE3-4F7F-8AC3-A8B3334B82A0}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{C9CD7770-2DB3-4C49-B6FA-5C73EE473DA6}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{4E3845B3-9ADE-400A-8865-93710519D3EB}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{5C8119D0-8F0A-49AA-ACCE-E6A330FF055D}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{6D2279F7-457D-4F72-BDB1-9287DA3CBD6D}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{4C606D41-237F-47A9-9C26-D7DCCF18D9A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup orientation="portrait" r:id="rId52"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F23" sqref="F23"/>
+      <selection pane="topRight" activeCell="A26" sqref="A26:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3122,30 +3229,110 @@
       <c r="AC25" s="8"/>
       <c r="AD25" s="6"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V26" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z26" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>319</v>
+      </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z27" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z29" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>320</v>
+      </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
+      <c r="X30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y30" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA30" s="12" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z31" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3154,7 +3341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3232,11 +3419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New scripts for Applicant Info.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA0FE4E-B752-4E06-A022-A9F3F661D30C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D037714-6ACF-4CA0-A99F-D81837F35466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="329">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1002,6 +1002,21 @@
     <t xml:space="preserve">
     By selecting Continue below you agree to not use any TDECU accounts, services or products for unlawful or illegal gambling practices in accordance with the Unlawful Internet Gambling Enforcement Act (UIGEA).
     </t>
+  </si>
+  <si>
+    <t>C23763_AddressShouldVerifiedForNonMemberUser</t>
+  </si>
+  <si>
+    <t>C23764_NonMemberUserShouldbeAbleToEnterStreetAddressAndZip</t>
+  </si>
+  <si>
+    <t>C23765_NonMemberUserCanSeeErrorMessageForInvalidDataEntry</t>
+  </si>
+  <si>
+    <t>C23794_NonMemberUserCanEnterPersonalIdentificationInfo</t>
+  </si>
+  <si>
+    <t>C23795_ApplicantInfoShouldDisplayedOnceReturnBackToThePage</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1191,7 +1206,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1395,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD53"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2220,23 +2235,78 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
+      <c r="A54" t="s">
+        <v>324</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
+      <c r="A55" t="s">
+        <v>325</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
+      <c r="A56" t="s">
+        <v>326</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
+      <c r="A57" t="s">
+        <v>327</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
+      <c r="A58" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2461,19 +2531,23 @@
     <hyperlink ref="B51" r:id="rId49" xr:uid="{5C8119D0-8F0A-49AA-ACCE-E6A330FF055D}"/>
     <hyperlink ref="B52" r:id="rId50" xr:uid="{6D2279F7-457D-4F72-BDB1-9287DA3CBD6D}"/>
     <hyperlink ref="B53" r:id="rId51" xr:uid="{4C606D41-237F-47A9-9C26-D7DCCF18D9A0}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{50714D4C-0E08-4895-B1DC-37A16FAC9F64}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{27AFFF6E-BE43-4972-B58D-807378C20682}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{5AEEAE7B-BD5E-4C30-815F-92B2321589AF}"/>
+    <hyperlink ref="B57" r:id="rId55" xr:uid="{39C303E1-EF85-448F-8DCA-FD2D7F3B9011}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{CDCB6377-12D4-4E1C-A01E-D91D7C00186A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId52"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD31"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H22" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3324,6 +3398,51 @@
       <c r="A31" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="X31" s="7" t="s">
         <v>80</v>
       </c>
@@ -3331,6 +3450,165 @@
         <v>85</v>
       </c>
       <c r="Z31" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>324</v>
+      </c>
+      <c r="X32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>325</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z33" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>326</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="X34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z34" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>327</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z35" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>328</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R36" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y36" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z36" s="7" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded new scripts of Applicant Info.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D037714-6ACF-4CA0-A99F-D81837F35466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629A7D1-D9F1-4067-8A55-0FC12503D69E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="338">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1017,6 +1017,33 @@
   </si>
   <si>
     <t>C23795_ApplicantInfoShouldDisplayedOnceReturnBackToThePage</t>
+  </si>
+  <si>
+    <t>C23796_NonMembersSSNAutometicallyFormatted</t>
+  </si>
+  <si>
+    <t>C23797_ApplicationProvideAlertForInvalidSSNEntries</t>
+  </si>
+  <si>
+    <t>C23799_ApplicationProvideAlertForInvalidDOBEntries</t>
+  </si>
+  <si>
+    <t>C23824_NonMemberUserCanEnterContactInformation</t>
+  </si>
+  <si>
+    <t>C23825_NonMemberUserGetAlertForInvalidPhoneNumberEntry</t>
+  </si>
+  <si>
+    <t>C23801_ApplicationProvideAlertForInvalidIssueDateEntries</t>
+  </si>
+  <si>
+    <t>C23803_ApplicationProvideAlertForInvalidExpirationDateEntries</t>
+  </si>
+  <si>
+    <t>C23826_NonMemberUserShouldAbletoSelectATypeOfEachPhoneNumber</t>
+  </si>
+  <si>
+    <t>C23827_NonMemberUserShouldGetAlertForInvalidEmailAddressEntry</t>
   </si>
 </sst>
 </file>
@@ -1410,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:D58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,97 +2337,196 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
+      <c r="A59" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="A60" t="s">
+        <v>330</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
+      <c r="A61" t="s">
+        <v>331</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="A62" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
+      <c r="A63" t="s">
+        <v>335</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
+      <c r="A64" t="s">
+        <v>332</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>333</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E65" s="2"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>336</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="E70" s="2"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="E76" s="2"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="E77" s="2"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="E78" s="2"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="F80" s="1"/>
     </row>
@@ -2536,18 +2662,27 @@
     <hyperlink ref="B56" r:id="rId54" xr:uid="{5AEEAE7B-BD5E-4C30-815F-92B2321589AF}"/>
     <hyperlink ref="B57" r:id="rId55" xr:uid="{39C303E1-EF85-448F-8DCA-FD2D7F3B9011}"/>
     <hyperlink ref="B58" r:id="rId56" xr:uid="{CDCB6377-12D4-4E1C-A01E-D91D7C00186A}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{BF9334EE-BBEE-4CCD-B448-0A85F57C76FD}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{7D1AEA6E-8EAB-4FD8-9BFA-4F0C13054F81}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{DA7D7F53-C32F-47CF-8EA2-9F7D99BA7CA2}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{3012E559-189F-4DF8-8DD3-7888AE1CCEED}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{0EB96C61-01BA-4859-AB77-50F0F1D76C53}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{F7A2A7C8-DAA9-4B09-BE43-B04D756A7936}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{69D62C08-7BA0-486B-AA13-20201E7330AC}"/>
+    <hyperlink ref="B66" r:id="rId64" xr:uid="{28BC49E4-3EC8-4C5E-B0EB-D352D6FFA1DC}"/>
+    <hyperlink ref="B67" r:id="rId65" xr:uid="{B0B5787F-6523-4472-8EF1-C4A813592DB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId57"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD36"/>
+  <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H22" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3467,7 +3602,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>325</v>
       </c>
@@ -3481,7 +3616,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>326</v>
       </c>
@@ -3506,7 +3641,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>327</v>
       </c>
@@ -3553,7 +3688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>328</v>
       </c>
@@ -3609,6 +3744,456 @@
         <v>85</v>
       </c>
       <c r="Z36" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>329</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y37" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z37" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R38" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U38" s="6"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y38" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z38" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>331</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z39" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>334</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P40" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R40" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U40" s="6"/>
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+      <c r="X40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y40" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z40" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P41" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R41" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S41" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z41" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>332</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U42" s="6"/>
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+      <c r="X42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z42" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA42" s="12" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>333</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z43" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>336</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X44" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y44" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z44" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>337</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P45" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R45" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y45" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z45" s="7" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new script and updated TestData & Locators.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD13B25E-BD03-4A7C-BA01-3806B297483B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB0CC9-E032-4136-ABEA-8A6B9C307157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="343">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1056,6 +1056,9 @@
   </si>
   <si>
     <t>600</t>
+  </si>
+  <si>
+    <t>C24259_NonMemberUserShouldAbleToReturnBackToThePreviousPage</t>
   </si>
 </sst>
 </file>
@@ -1449,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:XFD71"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,7 +2551,18 @@
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
+      <c r="A72" t="s">
+        <v>342</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2731,19 +2745,20 @@
     <hyperlink ref="B69" r:id="rId67" xr:uid="{102BD061-7CAB-426F-80A2-AEECCD517C93}"/>
     <hyperlink ref="B70" r:id="rId68" xr:uid="{596CEF63-52F0-46E8-BAC7-71A11B2EA888}"/>
     <hyperlink ref="B71" r:id="rId69" xr:uid="{BE37E8AA-F0B3-49C9-84AF-5673787A81F8}"/>
+    <hyperlink ref="B72" r:id="rId70" xr:uid="{754F1E95-0C2E-4196-BC79-4BD050B2CA94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId70"/>
+  <pageSetup orientation="portrait" r:id="rId71"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD49"/>
+  <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A46" sqref="A46:XFD49"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4460,7 +4475,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>339</v>
       </c>
@@ -4475,6 +4490,23 @@
       </c>
       <c r="Z49" s="7" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="X50" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y50" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z50" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA50" s="12" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New scripts added for Applicant Info
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB0CC9-E032-4136-ABEA-8A6B9C307157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC5AE2-BB6F-43F3-AE36-D7D3515E316D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="345">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1059,6 +1059,12 @@
   </si>
   <si>
     <t>C24259_NonMemberUserShouldAbleToReturnBackToThePreviousPage</t>
+  </si>
+  <si>
+    <t>C23935_NonMemberUserShouldAbleToEnterLoanInfo</t>
+  </si>
+  <si>
+    <t>C23938_NonMemberUserMustEnterValuesIfAppliedForLoanOrCreditCard</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1459,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+      <selection activeCell="B73" sqref="B73:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,11 +2572,33 @@
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
+      <c r="A73" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
+      <c r="A74" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2746,19 +2774,21 @@
     <hyperlink ref="B70" r:id="rId68" xr:uid="{596CEF63-52F0-46E8-BAC7-71A11B2EA888}"/>
     <hyperlink ref="B71" r:id="rId69" xr:uid="{BE37E8AA-F0B3-49C9-84AF-5673787A81F8}"/>
     <hyperlink ref="B72" r:id="rId70" xr:uid="{754F1E95-0C2E-4196-BC79-4BD050B2CA94}"/>
+    <hyperlink ref="B73" r:id="rId71" xr:uid="{507F6CA1-E8EA-4FEF-A5D8-BEB4DD252FFF}"/>
+    <hyperlink ref="B74" r:id="rId72" xr:uid="{4E207CDC-81C8-4B10-9A69-8CF5118EE0C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId71"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD50"/>
+  <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A50" sqref="A50:XFD50"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4509,6 +4539,130 @@
         <v>336</v>
       </c>
     </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>343</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R51" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S51" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T51" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U51" s="6"/>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z51" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>344</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T52" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U52" s="6"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y52" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z52" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New script added on ConfirmAccounts.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC5AE2-BB6F-43F3-AE36-D7D3515E316D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FBD820-6CBB-46DD-9D52-A6F27FE112D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="359">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1065,6 +1065,48 @@
   </si>
   <si>
     <t>C23938_NonMemberUserMustEnterValuesIfAppliedForLoanOrCreditCard</t>
+  </si>
+  <si>
+    <t>C23857_NonMemberUserWouldLikeToViewSelectedAccountInfo</t>
+  </si>
+  <si>
+    <t>AccountSelection</t>
+  </si>
+  <si>
+    <t>6 Month Share Certificate (Estimated Maturity Date: 6/13/2020)::High Yield Checking::Debit Card::Mobile Remote Deposit Capture::Online/Mobile Banking::E-Documents::MAXINE – Self-Service Telephone Banking</t>
+  </si>
+  <si>
+    <t>C23858_NonMemberUserWouldAddAccountBeforeConfirming</t>
+  </si>
+  <si>
+    <t>C23859_NonMemberUserWouldLikeToRemovePreSelectedOption</t>
+  </si>
+  <si>
+    <t>C23860_NonMemberUserWouldLikeToModifyAccountInfoBeforeConfirming</t>
+  </si>
+  <si>
+    <t>TestCompany</t>
+  </si>
+  <si>
+    <t>Test Automation Engineer</t>
+  </si>
+  <si>
+    <t>8008391146</t>
+  </si>
+  <si>
+    <t>C24228_NonMemberUserCanGetMobileDepositLinkIfOptionSelected</t>
+  </si>
+  <si>
+    <t>C23862_NonMemberUserCanVerifyTheIdentity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test@emailaddress.com</t>
+  </si>
+  <si>
+    <t>B-Company</t>
+  </si>
+  <si>
+    <t>7008391159</t>
   </si>
 </sst>
 </file>
@@ -1458,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73:D74"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2602,30 +2644,96 @@
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
+      <c r="A75" t="s">
+        <v>345</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
+      <c r="A76" t="s">
+        <v>348</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E76" s="2"/>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="4"/>
+      <c r="A77" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E77" s="2"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
+      <c r="A78" t="s">
+        <v>350</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E78" s="2"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
+      <c r="A79" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
+      <c r="A80" t="s">
+        <v>355</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
@@ -2776,19 +2884,25 @@
     <hyperlink ref="B72" r:id="rId70" xr:uid="{754F1E95-0C2E-4196-BC79-4BD050B2CA94}"/>
     <hyperlink ref="B73" r:id="rId71" xr:uid="{507F6CA1-E8EA-4FEF-A5D8-BEB4DD252FFF}"/>
     <hyperlink ref="B74" r:id="rId72" xr:uid="{4E207CDC-81C8-4B10-9A69-8CF5118EE0C0}"/>
+    <hyperlink ref="B75" r:id="rId73" xr:uid="{9C24E18F-3DCE-4084-AE08-BC613DF917E4}"/>
+    <hyperlink ref="B76" r:id="rId74" xr:uid="{746A6E87-38A4-4ADB-9E01-7F847D47986E}"/>
+    <hyperlink ref="B77" r:id="rId75" xr:uid="{494C7915-33E8-48F2-AD37-DAEE4196EF34}"/>
+    <hyperlink ref="B78" r:id="rId76" xr:uid="{693DAA6D-4D01-425F-A177-14FC0D044266}"/>
+    <hyperlink ref="B79" r:id="rId77" xr:uid="{23C01B26-6919-4A21-8998-910403C2B9A7}"/>
+    <hyperlink ref="B80" r:id="rId78" xr:uid="{A1B321FB-A764-4F44-994A-27B1DCEB1823}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD52"/>
+  <dimension ref="A1:AD58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q58" sqref="Q58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,9 +2928,10 @@
     <col min="27" max="27" width="64.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="193.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2904,8 +3019,11 @@
       <c r="AC1" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD1" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2962,7 +3080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2979,7 +3097,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>48</v>
       </c>
@@ -2996,7 +3114,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -3019,7 +3137,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
@@ -3036,7 +3154,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -3056,7 +3174,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
@@ -3076,7 +3194,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -3084,7 +3202,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -3104,7 +3222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -3124,7 +3242,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -3143,7 +3261,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -3158,7 +3276,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>92</v>
       </c>
@@ -3172,7 +3290,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -3186,7 +3304,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -4505,7 +4623,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>339</v>
       </c>
@@ -4522,7 +4640,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>342</v>
       </c>
@@ -4539,7 +4657,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>343</v>
       </c>
@@ -4601,7 +4719,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>344</v>
       </c>
@@ -4660,6 +4778,400 @@
         <v>85</v>
       </c>
       <c r="Z52" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R53" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T53" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y53" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z53" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P54" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S54" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+      <c r="X54" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y54" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z54" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA54" s="6"/>
+      <c r="AB54" s="6"/>
+      <c r="AC54" s="6"/>
+      <c r="AD54" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>349</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P55" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S55" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U55" s="6"/>
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+      <c r="X55" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y55" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z55" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA55" s="6"/>
+      <c r="AB55" s="6"/>
+      <c r="AC55" s="6"/>
+      <c r="AD55" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="P56" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S56" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U56" s="6"/>
+      <c r="V56" s="6"/>
+      <c r="W56" s="6"/>
+      <c r="X56" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y56" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z56" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA56" s="6"/>
+      <c r="AB56" s="6"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>354</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S57" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U57" s="6"/>
+      <c r="V57" s="6"/>
+      <c r="W57" s="6"/>
+      <c r="X57" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y57" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z57" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA57" s="6"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>355</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P58" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R58" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S58" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y58" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z58" s="7" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added IdentityVerification and modification done.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FBD820-6CBB-46DD-9D52-A6F27FE112D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA866FE-114D-4FE1-A491-A39F7B9CF125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="363">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1107,6 +1107,18 @@
   </si>
   <si>
     <t>7008391159</t>
+  </si>
+  <si>
+    <t>8008391256</t>
+  </si>
+  <si>
+    <t>9875675</t>
+  </si>
+  <si>
+    <t>C24271_NonMemberUserWouldLikeToSeeNoneOfTheAboveAsanAnswer</t>
+  </si>
+  <si>
+    <t>9875687</t>
   </si>
 </sst>
 </file>
@@ -1500,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79:D80"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80:D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,73 +2748,84 @@
       </c>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="E84" s="2"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="E85" s="2"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="E86" s="2"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="E87" s="2"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="E88" s="2"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="E89" s="2"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="F96" s="1"/>
     </row>
@@ -2890,19 +2913,20 @@
     <hyperlink ref="B78" r:id="rId76" xr:uid="{693DAA6D-4D01-425F-A177-14FC0D044266}"/>
     <hyperlink ref="B79" r:id="rId77" xr:uid="{23C01B26-6919-4A21-8998-910403C2B9A7}"/>
     <hyperlink ref="B80" r:id="rId78" xr:uid="{A1B321FB-A764-4F44-994A-27B1DCEB1823}"/>
+    <hyperlink ref="B81" r:id="rId79" xr:uid="{91A1449C-A6E6-4898-83FD-D46FD7803DF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId79"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD58"/>
+  <dimension ref="A1:AD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q58" sqref="Q58"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4925,7 +4949,7 @@
         <v>29</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>45</v>
+        <v>360</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>46</v>
@@ -4946,13 +4970,13 @@
         <v>41</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>38</v>
+        <v>351</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>30</v>
+        <v>352</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>31</v>
+        <v>359</v>
       </c>
       <c r="R55" s="6" t="s">
         <v>32</v>
@@ -5174,6 +5198,71 @@
       <c r="Z58" s="7" t="s">
         <v>82</v>
       </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>361</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P59" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S59" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y59" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z59" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA59" s="6"/>
+      <c r="AB59" s="6"/>
+      <c r="AC59" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added, JointOwners and E-Doc scripts.
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA866FE-114D-4FE1-A491-A39F7B9CF125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5B83F7-0757-452E-9901-F98B8C2573CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="371">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1119,6 +1119,30 @@
   </si>
   <si>
     <t>9875687</t>
+  </si>
+  <si>
+    <t>C24263_NonMemberUserCanOnlySeeEDocumentLinkIfSelected</t>
+  </si>
+  <si>
+    <t>9875677</t>
+  </si>
+  <si>
+    <t>C24264_NonMemberUserShouldNotSeeEDocumentLinkIfNotSelected</t>
+  </si>
+  <si>
+    <t>C23939_NonMemberUserShouldFillEntireApplicantFormMustBeCompletedBeforeProcced</t>
+  </si>
+  <si>
+    <t>C23941_NonMemberUserShouldFillEntireApplicantFormMustBeCompletedBeforeProccedWithAddBeneFiciaries</t>
+  </si>
+  <si>
+    <t>C23942_NonMemberUserCanAddOneJointOwnerToTheApplicationForm</t>
+  </si>
+  <si>
+    <t>9875668</t>
+  </si>
+  <si>
+    <t>9875676</t>
   </si>
 </sst>
 </file>
@@ -1512,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80:D81"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,25 +2788,80 @@
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
+      <c r="A82" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+      <c r="A83" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
+      <c r="A84" t="s">
+        <v>366</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E84" s="2"/>
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
+      <c r="A85" t="s">
+        <v>367</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E85" s="2"/>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
+      <c r="A86" t="s">
+        <v>368</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E86" s="2"/>
       <c r="F86" s="1"/>
     </row>
@@ -2914,24 +2993,29 @@
     <hyperlink ref="B79" r:id="rId77" xr:uid="{23C01B26-6919-4A21-8998-910403C2B9A7}"/>
     <hyperlink ref="B80" r:id="rId78" xr:uid="{A1B321FB-A764-4F44-994A-27B1DCEB1823}"/>
     <hyperlink ref="B81" r:id="rId79" xr:uid="{91A1449C-A6E6-4898-83FD-D46FD7803DF6}"/>
+    <hyperlink ref="B82" r:id="rId80" xr:uid="{F9FC268B-5594-4802-8F1E-61C01EBE9077}"/>
+    <hyperlink ref="B83" r:id="rId81" xr:uid="{1D9B8076-AECC-44DD-824F-99C1E52C83D3}"/>
+    <hyperlink ref="B84" r:id="rId82" xr:uid="{7CD31FAC-166B-4C80-B840-5B5DFDF33964}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{583BD021-50FC-45E2-8E9E-4B14C4C2A0E1}"/>
+    <hyperlink ref="B86" r:id="rId84" xr:uid="{47C965E7-2448-4F2C-87D3-9A571567D6AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId80"/>
+  <pageSetup orientation="portrait" r:id="rId85"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD59"/>
+  <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="103" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
@@ -2945,6 +3029,7 @@
     <col min="15" max="15" width="17.28515625" customWidth="1"/>
     <col min="17" max="17" width="12.42578125" customWidth="1"/>
     <col min="19" max="19" width="23.28515625" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="54.140625" customWidth="1"/>
@@ -5263,6 +5348,219 @@
       <c r="AA59" s="6"/>
       <c r="AB59" s="6"/>
       <c r="AC59" s="6"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>363</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R60" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S60" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X60" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y60" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z60" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>365</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P61" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R61" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S61" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+      <c r="W61" s="6"/>
+      <c r="X61" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y61" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z61" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="X62" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y62" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z62" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>367</v>
+      </c>
+      <c r="X63" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y63" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z63" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O64" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P64" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q64" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R64" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S64" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T64" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U64" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="V64" s="6"/>
+      <c r="W64" s="6"/>
+      <c r="X64" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y64" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z64" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Member Agreement and Disclosures scripts
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5B83F7-0757-452E-9901-F98B8C2573CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="DNA_Upgrade" sheetId="3" r:id="rId3"/>
     <sheet name="ProdData" sheetId="4" r:id="rId4"/>
+    <sheet name="DataTwo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="434">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1143,12 +1143,201 @@
   </si>
   <si>
     <t>9875676</t>
+  </si>
+  <si>
+    <t>DescText1</t>
+  </si>
+  <si>
+    <t>DescText2</t>
+  </si>
+  <si>
+    <t>DescText3</t>
+  </si>
+  <si>
+    <t>DescText4</t>
+  </si>
+  <si>
+    <t>DescText5</t>
+  </si>
+  <si>
+    <t>DescText6</t>
+  </si>
+  <si>
+    <t>DescText7</t>
+  </si>
+  <si>
+    <t>DescText8</t>
+  </si>
+  <si>
+    <t>DescText9</t>
+  </si>
+  <si>
+    <t>DescText10</t>
+  </si>
+  <si>
+    <t>DescText11</t>
+  </si>
+  <si>
+    <t>DescText12</t>
+  </si>
+  <si>
+    <t>DescText13</t>
+  </si>
+  <si>
+    <t>C24290_VerifyCourtesyPayAgreements</t>
+  </si>
+  <si>
+    <t>02/02/1950</t>
+  </si>
+  <si>
+    <t>Test-1000</t>
+  </si>
+  <si>
+    <t>02/02/2012</t>
+  </si>
+  <si>
+    <t>02/02/2025</t>
+  </si>
+  <si>
+    <t>Mname</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>test+1@email.com</t>
+  </si>
+  <si>
+    <t>TDECU provides several overdraft protection options on your checking account to protect you from having items returned due to insufficient funds. An overdraft occurs when the available balance in your account is insufficient to cover a transaction, but we pay it anyway. We can cover your overdrafts in three ways:</t>
+  </si>
+  <si>
+    <t>Automatic transfers from available funds in your savings account to your checking account.</t>
+  </si>
+  <si>
+    <t>Automatic transfers from available funds in your Cash Stash line of credit to your checking account</t>
+  </si>
+  <si>
+    <t>We also offer standard overdraft practices that come with your account, which we refer to as Courtesy Pay, which allows us to overdraw your checking account in order to pay a transaction up to a predetermined limit. Currently, this can be used to cover checks, debit card purchases, ATM withdrawals, and ACH transactions.</t>
+  </si>
+  <si>
+    <t>Federal regulations require new checking account holders to opt in to Courtesy Pay if you want to have the overdraft of ATM and one-time debit transactions covered.</t>
+  </si>
+  <si>
+    <t>What are the standard overdraft practices that come with my account?</t>
+  </si>
+  <si>
+    <t>What fees will I be charged if TDECU pays my overdraft?</t>
+  </si>
+  <si>
+    <t>We will charge you a $32 fee each time we pay an overdraft. There is no limit on the total fees we can charge you for overdrawing your account. However, there is no fee for overdraft transfers from your savings account.</t>
+  </si>
+  <si>
+    <t>NOTE: Courtesy Pay will be activated after your checking account has been open for 60 days and if the account is in good standing. Please see the Account Information Brochure for more information regarding Courtesy Pay.</t>
+  </si>
+  <si>
+    <t>C24265_VerifyAgreementsandDisclosures</t>
+  </si>
+  <si>
+    <t>01/01/1960</t>
+  </si>
+  <si>
+    <t>test+3@email.com</t>
+  </si>
+  <si>
+    <t>Please accept the disclosures.</t>
+  </si>
+  <si>
+    <t>By clicking this box, I acknowledge that I have reviewed and agree to the terms and conditions of the above disclosures. I acknowledge that the primary account owner and any joint owners of this account will be bound by such disclosures. I understand I can obtain copies of the disclosures at any Member Center, by calling Member Care at (800) 839-1154, or by visiting tdecu.org.</t>
+  </si>
+  <si>
+    <t>The number I have entered is my correct taxpayer identification number.</t>
+  </si>
+  <si>
+    <t>Taxpayer Identification Number (TIN): The number I have entered is my correct taxpayer identification number.</t>
+  </si>
+  <si>
+    <t>You must select that you are not subject to backup withholding or that you are an exempt recipient under the Internal Revenue Service Regulations.</t>
+  </si>
+  <si>
+    <t>I am not subject to backup withholding either because I have not been notified that I am subject to backup withholding as a result of a failure to report all interest or dividends, or the Internal Revenue Service has notified me that I am no longer subject to backup withholding.</t>
+  </si>
+  <si>
+    <t>Exempt Recipients: I am an exempt recipient under the Internal Revenue Service Regulations.</t>
+  </si>
+  <si>
+    <t>Are you a US Citizen or a Non-Resident Alien?</t>
+  </si>
+  <si>
+    <t>I certify under penalties of perjury the statements checked in this section and that I am a U.S. person (including a U. S. resident alien).</t>
+  </si>
+  <si>
+    <t>I certify that I am a non-resident alien and understand that I must complete and keep on file a current IRS Form W-8BEN.</t>
+  </si>
+  <si>
+    <t>Please complete the Agreement and Signatures section to continue.</t>
+  </si>
+  <si>
+    <t>I authorize TDECU to investigate my credit and employment history and obtain reports from consumer reporting agency(ies) to determine if it should open my account. The undersigned, jointly and severally, agree to the bylaws of TDECU, including any requirement to pay a membership or entrance fee, and agree to the terms of, and acknowledge receipt of electronic copy(ies) of, this document.</t>
+  </si>
+  <si>
+    <t>By clicking the "ACCEPT" button, I attest to this as my legally binding signature and that I acknowledge that I have reviewed and agreed to the terms and conditions for the above disclosures. If I do not agree to any of this, I understand that I do not need to move forward with the application.</t>
+  </si>
+  <si>
+    <t>C24266_VerifyDeclineAgreements</t>
+  </si>
+  <si>
+    <t>03/03/1970</t>
+  </si>
+  <si>
+    <t>test+2@email.com</t>
+  </si>
+  <si>
+    <t>C24297_VerifySelectOneTaxOption</t>
+  </si>
+  <si>
+    <t>04/04/1980</t>
+  </si>
+  <si>
+    <t>test+4@email.com</t>
+  </si>
+  <si>
+    <t>Please select only one backup withholding option.</t>
+  </si>
+  <si>
+    <t>C24298_VerifySelectOneResidentOption</t>
+  </si>
+  <si>
+    <t>05/05/1990</t>
+  </si>
+  <si>
+    <t>test+5@email.com</t>
+  </si>
+  <si>
+    <t>Please select if you are a U.S. Citizen or non-Resident Alien.</t>
+  </si>
+  <si>
+    <t>51422589</t>
+  </si>
+  <si>
+    <t>35688741</t>
+  </si>
+  <si>
+    <t>42355698</t>
+  </si>
+  <si>
+    <t>65211025</t>
+  </si>
+  <si>
+    <t>45688741</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1533,11 +1722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,26 +3055,81 @@
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
+      <c r="A87" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E87" s="2"/>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+      <c r="A88" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E88" s="2"/>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+      <c r="A89" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+      <c r="A90" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
+      <c r="A91" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2914,102 +3158,107 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B48" r:id="rId46" xr:uid="{2C6782D2-E315-48D4-B754-2228BA2B308E}"/>
-    <hyperlink ref="B49" r:id="rId47" xr:uid="{2038515E-2630-43E9-9273-7EED0BBF7995}"/>
-    <hyperlink ref="B50" r:id="rId48" xr:uid="{6BC67AE2-5B9C-475B-873C-3DE821FC3592}"/>
-    <hyperlink ref="B51" r:id="rId49" xr:uid="{2502A74E-9EA6-4229-9BA7-42F046F2356B}"/>
-    <hyperlink ref="B52" r:id="rId50" xr:uid="{85D83142-425A-4BBD-A48A-4264F864F9B6}"/>
-    <hyperlink ref="B53" r:id="rId51" xr:uid="{FEB5A26E-13D3-438F-8BD6-C63C81021A29}"/>
-    <hyperlink ref="B54" r:id="rId52" xr:uid="{2A672BE0-6FFC-4748-820E-6E82715BB76C}"/>
-    <hyperlink ref="B55" r:id="rId53" xr:uid="{1B9391F6-C91C-4A88-B536-AEB7B59017A8}"/>
-    <hyperlink ref="B56" r:id="rId54" xr:uid="{6C227A5B-6C72-4F0C-B346-FD0FB92D74DE}"/>
-    <hyperlink ref="B57" r:id="rId55" xr:uid="{AFFFEEBB-7A75-44A4-962C-72A080A75462}"/>
-    <hyperlink ref="B58" r:id="rId56" xr:uid="{D49FF145-CC56-4FFF-A554-BB4857C7432A}"/>
-    <hyperlink ref="B59" r:id="rId57" xr:uid="{ECA53405-D8E9-4166-B9C3-79BA8198623B}"/>
-    <hyperlink ref="B60" r:id="rId58" xr:uid="{A351FA5D-82F1-48EA-A236-0B6FF2EB72BB}"/>
-    <hyperlink ref="B61" r:id="rId59" xr:uid="{ABCFB80B-B2F5-4644-8337-D66215AA7AAF}"/>
-    <hyperlink ref="B62" r:id="rId60" xr:uid="{AEAE3612-B26F-4C1E-8113-F25ED9D51FF6}"/>
-    <hyperlink ref="B63" r:id="rId61" xr:uid="{7157AF5D-5CE8-4C50-815C-C6F6D841964A}"/>
-    <hyperlink ref="B64" r:id="rId62" xr:uid="{EA9D85A0-D97F-4AA1-A7E4-836D0F2621B7}"/>
-    <hyperlink ref="B65" r:id="rId63" xr:uid="{CF8D253A-7F8B-4B61-B04D-380EB3B59231}"/>
-    <hyperlink ref="B66" r:id="rId64" xr:uid="{4B727B1E-5279-4345-B01C-4F737F3BF4D7}"/>
-    <hyperlink ref="B67" r:id="rId65" xr:uid="{D81FD3C9-15F3-4198-A96E-140F369AADA2}"/>
-    <hyperlink ref="B68" r:id="rId66" xr:uid="{92ED9EEC-F5C1-47C1-B051-449C9165FF7D}"/>
-    <hyperlink ref="B69" r:id="rId67" xr:uid="{102BD061-7CAB-426F-80A2-AEECCD517C93}"/>
-    <hyperlink ref="B70" r:id="rId68" xr:uid="{596CEF63-52F0-46E8-BAC7-71A11B2EA888}"/>
-    <hyperlink ref="B71" r:id="rId69" xr:uid="{BE37E8AA-F0B3-49C9-84AF-5673787A81F8}"/>
-    <hyperlink ref="B72" r:id="rId70" xr:uid="{754F1E95-0C2E-4196-BC79-4BD050B2CA94}"/>
-    <hyperlink ref="B73" r:id="rId71" xr:uid="{507F6CA1-E8EA-4FEF-A5D8-BEB4DD252FFF}"/>
-    <hyperlink ref="B74" r:id="rId72" xr:uid="{4E207CDC-81C8-4B10-9A69-8CF5118EE0C0}"/>
-    <hyperlink ref="B75" r:id="rId73" xr:uid="{9C24E18F-3DCE-4084-AE08-BC613DF917E4}"/>
-    <hyperlink ref="B76" r:id="rId74" xr:uid="{746A6E87-38A4-4ADB-9E01-7F847D47986E}"/>
-    <hyperlink ref="B77" r:id="rId75" xr:uid="{494C7915-33E8-48F2-AD37-DAEE4196EF34}"/>
-    <hyperlink ref="B78" r:id="rId76" xr:uid="{693DAA6D-4D01-425F-A177-14FC0D044266}"/>
-    <hyperlink ref="B79" r:id="rId77" xr:uid="{23C01B26-6919-4A21-8998-910403C2B9A7}"/>
-    <hyperlink ref="B80" r:id="rId78" xr:uid="{A1B321FB-A764-4F44-994A-27B1DCEB1823}"/>
-    <hyperlink ref="B81" r:id="rId79" xr:uid="{91A1449C-A6E6-4898-83FD-D46FD7803DF6}"/>
-    <hyperlink ref="B82" r:id="rId80" xr:uid="{F9FC268B-5594-4802-8F1E-61C01EBE9077}"/>
-    <hyperlink ref="B83" r:id="rId81" xr:uid="{1D9B8076-AECC-44DD-824F-99C1E52C83D3}"/>
-    <hyperlink ref="B84" r:id="rId82" xr:uid="{7CD31FAC-166B-4C80-B840-5B5DFDF33964}"/>
-    <hyperlink ref="B85" r:id="rId83" xr:uid="{583BD021-50FC-45E2-8E9E-4B14C4C2A0E1}"/>
-    <hyperlink ref="B86" r:id="rId84" xr:uid="{47C965E7-2448-4F2C-87D3-9A571567D6AA}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B20" r:id="rId18"/>
+    <hyperlink ref="B21" r:id="rId19"/>
+    <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B23" r:id="rId21"/>
+    <hyperlink ref="B24" r:id="rId22"/>
+    <hyperlink ref="B25" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
+    <hyperlink ref="B27" r:id="rId25"/>
+    <hyperlink ref="B28" r:id="rId26"/>
+    <hyperlink ref="B29" r:id="rId27"/>
+    <hyperlink ref="B30" r:id="rId28"/>
+    <hyperlink ref="B31" r:id="rId29"/>
+    <hyperlink ref="B32" r:id="rId30"/>
+    <hyperlink ref="B33" r:id="rId31"/>
+    <hyperlink ref="B34" r:id="rId32"/>
+    <hyperlink ref="B35" r:id="rId33"/>
+    <hyperlink ref="B36" r:id="rId34"/>
+    <hyperlink ref="B37" r:id="rId35"/>
+    <hyperlink ref="B38" r:id="rId36"/>
+    <hyperlink ref="B39" r:id="rId37"/>
+    <hyperlink ref="B40" r:id="rId38"/>
+    <hyperlink ref="B41" r:id="rId39"/>
+    <hyperlink ref="B42" r:id="rId40"/>
+    <hyperlink ref="B43" r:id="rId41"/>
+    <hyperlink ref="B44" r:id="rId42"/>
+    <hyperlink ref="B45" r:id="rId43"/>
+    <hyperlink ref="B46" r:id="rId44"/>
+    <hyperlink ref="B47" r:id="rId45"/>
+    <hyperlink ref="B48" r:id="rId46"/>
+    <hyperlink ref="B49" r:id="rId47"/>
+    <hyperlink ref="B50" r:id="rId48"/>
+    <hyperlink ref="B51" r:id="rId49"/>
+    <hyperlink ref="B52" r:id="rId50"/>
+    <hyperlink ref="B53" r:id="rId51"/>
+    <hyperlink ref="B54" r:id="rId52"/>
+    <hyperlink ref="B55" r:id="rId53"/>
+    <hyperlink ref="B56" r:id="rId54"/>
+    <hyperlink ref="B57" r:id="rId55"/>
+    <hyperlink ref="B58" r:id="rId56"/>
+    <hyperlink ref="B59" r:id="rId57"/>
+    <hyperlink ref="B60" r:id="rId58"/>
+    <hyperlink ref="B61" r:id="rId59"/>
+    <hyperlink ref="B62" r:id="rId60"/>
+    <hyperlink ref="B63" r:id="rId61"/>
+    <hyperlink ref="B64" r:id="rId62"/>
+    <hyperlink ref="B65" r:id="rId63"/>
+    <hyperlink ref="B66" r:id="rId64"/>
+    <hyperlink ref="B67" r:id="rId65"/>
+    <hyperlink ref="B68" r:id="rId66"/>
+    <hyperlink ref="B69" r:id="rId67"/>
+    <hyperlink ref="B70" r:id="rId68"/>
+    <hyperlink ref="B71" r:id="rId69"/>
+    <hyperlink ref="B72" r:id="rId70"/>
+    <hyperlink ref="B73" r:id="rId71"/>
+    <hyperlink ref="B74" r:id="rId72"/>
+    <hyperlink ref="B75" r:id="rId73"/>
+    <hyperlink ref="B76" r:id="rId74"/>
+    <hyperlink ref="B77" r:id="rId75"/>
+    <hyperlink ref="B78" r:id="rId76"/>
+    <hyperlink ref="B79" r:id="rId77"/>
+    <hyperlink ref="B80" r:id="rId78"/>
+    <hyperlink ref="B81" r:id="rId79"/>
+    <hyperlink ref="B82" r:id="rId80"/>
+    <hyperlink ref="B83" r:id="rId81"/>
+    <hyperlink ref="B84" r:id="rId82"/>
+    <hyperlink ref="B85" r:id="rId83"/>
+    <hyperlink ref="B86" r:id="rId84"/>
+    <hyperlink ref="B87" r:id="rId85"/>
+    <hyperlink ref="B88" r:id="rId86"/>
+    <hyperlink ref="B89" r:id="rId87"/>
+    <hyperlink ref="B90" r:id="rId88"/>
+    <hyperlink ref="B91" r:id="rId89"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId85"/>
+  <pageSetup orientation="portrait" r:id="rId90"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
@@ -5569,7 +5818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5647,7 +5896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6753,4 +7002,466 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6"/>
+    <col min="6" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="6"/>
+    <col min="15" max="15" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="6"/>
+    <col min="18" max="18" width="18" style="6" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="23.85546875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" style="6" customWidth="1"/>
+    <col min="22" max="22" width="24" style="6" customWidth="1"/>
+    <col min="23" max="23" width="25.42578125" style="6" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="6" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" style="6" customWidth="1"/>
+    <col min="26" max="26" width="18.85546875" style="6" customWidth="1"/>
+    <col min="27" max="27" width="20.42578125" style="6" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" style="6" customWidth="1"/>
+    <col min="29" max="29" width="18.28515625" style="6" customWidth="1"/>
+    <col min="30" max="30" width="22.140625" style="6" customWidth="1"/>
+    <col min="31" max="31" width="29.7109375" style="6" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>428</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Scripts added to JointAccount/Beneficiary
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7C985-DC43-4A87-88AE-FFF049902205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="444">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1332,12 +1333,42 @@
   </si>
   <si>
     <t>45688741</t>
+  </si>
+  <si>
+    <t>C23943_NonMemberUserCanAddMultipleJointOwnerToTheApplicationForm</t>
+  </si>
+  <si>
+    <t>9875568</t>
+  </si>
+  <si>
+    <t>9575676</t>
+  </si>
+  <si>
+    <t>9875758</t>
+  </si>
+  <si>
+    <t>C23944_NonMemberUserCanAddOneBeneficiaryToTheApplicationForm</t>
+  </si>
+  <si>
+    <t>9675668</t>
+  </si>
+  <si>
+    <t>9675677</t>
+  </si>
+  <si>
+    <t>9578676</t>
+  </si>
+  <si>
+    <t>C23945_NonMemberUserCanAddMultipleBeneficiariesToTheApplicationForm</t>
+  </si>
+  <si>
+    <t>9675758</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1722,11 +1753,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91:D91"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93:D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,9 +3085,9 @@
       <c r="E86" s="2"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>384</v>
+    <row r="87" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>434</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>8</v>
@@ -3072,7 +3103,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>8</v>
@@ -3088,7 +3119,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>8</v>
@@ -3104,7 +3135,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>8</v>
@@ -3115,33 +3146,67 @@
       <c r="D90" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="E90" s="2"/>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
+      <c r="B92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+      <c r="A93" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="A94" t="s">
+        <v>442</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3156,110 +3221,117 @@
       <c r="B97" s="4"/>
       <c r="F97" s="1"/>
     </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+      <c r="F98" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
-    <hyperlink ref="B23" r:id="rId21"/>
-    <hyperlink ref="B24" r:id="rId22"/>
-    <hyperlink ref="B25" r:id="rId23"/>
-    <hyperlink ref="B26" r:id="rId24"/>
-    <hyperlink ref="B27" r:id="rId25"/>
-    <hyperlink ref="B28" r:id="rId26"/>
-    <hyperlink ref="B29" r:id="rId27"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B31" r:id="rId29"/>
-    <hyperlink ref="B32" r:id="rId30"/>
-    <hyperlink ref="B33" r:id="rId31"/>
-    <hyperlink ref="B34" r:id="rId32"/>
-    <hyperlink ref="B35" r:id="rId33"/>
-    <hyperlink ref="B36" r:id="rId34"/>
-    <hyperlink ref="B37" r:id="rId35"/>
-    <hyperlink ref="B38" r:id="rId36"/>
-    <hyperlink ref="B39" r:id="rId37"/>
-    <hyperlink ref="B40" r:id="rId38"/>
-    <hyperlink ref="B41" r:id="rId39"/>
-    <hyperlink ref="B42" r:id="rId40"/>
-    <hyperlink ref="B43" r:id="rId41"/>
-    <hyperlink ref="B44" r:id="rId42"/>
-    <hyperlink ref="B45" r:id="rId43"/>
-    <hyperlink ref="B46" r:id="rId44"/>
-    <hyperlink ref="B47" r:id="rId45"/>
-    <hyperlink ref="B48" r:id="rId46"/>
-    <hyperlink ref="B49" r:id="rId47"/>
-    <hyperlink ref="B50" r:id="rId48"/>
-    <hyperlink ref="B51" r:id="rId49"/>
-    <hyperlink ref="B52" r:id="rId50"/>
-    <hyperlink ref="B53" r:id="rId51"/>
-    <hyperlink ref="B54" r:id="rId52"/>
-    <hyperlink ref="B55" r:id="rId53"/>
-    <hyperlink ref="B56" r:id="rId54"/>
-    <hyperlink ref="B57" r:id="rId55"/>
-    <hyperlink ref="B58" r:id="rId56"/>
-    <hyperlink ref="B59" r:id="rId57"/>
-    <hyperlink ref="B60" r:id="rId58"/>
-    <hyperlink ref="B61" r:id="rId59"/>
-    <hyperlink ref="B62" r:id="rId60"/>
-    <hyperlink ref="B63" r:id="rId61"/>
-    <hyperlink ref="B64" r:id="rId62"/>
-    <hyperlink ref="B65" r:id="rId63"/>
-    <hyperlink ref="B66" r:id="rId64"/>
-    <hyperlink ref="B67" r:id="rId65"/>
-    <hyperlink ref="B68" r:id="rId66"/>
-    <hyperlink ref="B69" r:id="rId67"/>
-    <hyperlink ref="B70" r:id="rId68"/>
-    <hyperlink ref="B71" r:id="rId69"/>
-    <hyperlink ref="B72" r:id="rId70"/>
-    <hyperlink ref="B73" r:id="rId71"/>
-    <hyperlink ref="B74" r:id="rId72"/>
-    <hyperlink ref="B75" r:id="rId73"/>
-    <hyperlink ref="B76" r:id="rId74"/>
-    <hyperlink ref="B77" r:id="rId75"/>
-    <hyperlink ref="B78" r:id="rId76"/>
-    <hyperlink ref="B79" r:id="rId77"/>
-    <hyperlink ref="B80" r:id="rId78"/>
-    <hyperlink ref="B81" r:id="rId79"/>
-    <hyperlink ref="B82" r:id="rId80"/>
-    <hyperlink ref="B83" r:id="rId81"/>
-    <hyperlink ref="B84" r:id="rId82"/>
-    <hyperlink ref="B85" r:id="rId83"/>
-    <hyperlink ref="B86" r:id="rId84"/>
-    <hyperlink ref="B87" r:id="rId85"/>
-    <hyperlink ref="B88" r:id="rId86"/>
-    <hyperlink ref="B89" r:id="rId87"/>
-    <hyperlink ref="B90" r:id="rId88"/>
-    <hyperlink ref="B91" r:id="rId89"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B87" r:id="rId90" xr:uid="{67E85579-CD16-4DCC-A3F6-C6653F801D89}"/>
+    <hyperlink ref="B93" r:id="rId91" xr:uid="{5EF7A279-F237-497D-B6E1-08B29D7CDC08}"/>
+    <hyperlink ref="B94" r:id="rId92" xr:uid="{B7687CFA-7998-4504-9E18-9B1BA1862F1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId90"/>
+  <pageSetup orientation="portrait" r:id="rId93"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
+      <selection pane="bottomLeft" activeCell="V67" sqref="V67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5811,6 +5883,202 @@
         <v>82</v>
       </c>
     </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>434</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O65" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P65" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q65" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R65" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S65" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T65" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U65" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="V65" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="W65" s="6"/>
+      <c r="X65" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y65" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z65" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>438</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O66" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P66" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q66" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R66" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S66" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T66" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U66" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y66" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z66" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>442</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O67" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P67" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q67" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R67" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S67" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T67" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U67" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="V67" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="W67" s="6"/>
+      <c r="X67" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y67" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z67" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5818,7 +6086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5896,7 +6164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7005,10 +7273,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New Member Beneficiary Role scripts
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7C985-DC43-4A87-88AE-FFF049902205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="482">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1363,12 +1362,126 @@
   </si>
   <si>
     <t>9675758</t>
+  </si>
+  <si>
+    <t>C24336_NonMemberBeneficiarySavingsRole</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>46889712</t>
+  </si>
+  <si>
+    <t>06/06/1955</t>
+  </si>
+  <si>
+    <t>test+6@email.com</t>
+  </si>
+  <si>
+    <t>512365541</t>
+  </si>
+  <si>
+    <t>C24335_NonMemberJOLoanandCCRoles</t>
+  </si>
+  <si>
+    <t>07/07/1965</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Barb</t>
+  </si>
+  <si>
+    <t>Henson</t>
+  </si>
+  <si>
+    <t>522365541</t>
+  </si>
+  <si>
+    <t>Classic MasterCard</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>C24334_NonMemberBeneficiaryMMRole</t>
+  </si>
+  <si>
+    <t>532365541</t>
+  </si>
+  <si>
+    <t>48889712</t>
+  </si>
+  <si>
+    <t>08/08/1975</t>
+  </si>
+  <si>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>test+7@email.com</t>
+  </si>
+  <si>
+    <t>test+8@email.com</t>
+  </si>
+  <si>
+    <t>52422589</t>
+  </si>
+  <si>
+    <t>C24333_NonMemberBeneficiaryCDRole</t>
+  </si>
+  <si>
+    <t>49889712</t>
+  </si>
+  <si>
+    <t>09/09/1985</t>
+  </si>
+  <si>
+    <t>542365541</t>
+  </si>
+  <si>
+    <t>Todd</t>
+  </si>
+  <si>
+    <t>Lambert</t>
+  </si>
+  <si>
+    <t>C24332_NonMemberBeneficiaryPersonalLoanRole</t>
+  </si>
+  <si>
+    <t>552365541</t>
+  </si>
+  <si>
+    <t>test+9@email.com</t>
+  </si>
+  <si>
+    <t>test@email.com</t>
+  </si>
+  <si>
+    <t>53422589</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Colt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1753,11 +1866,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93:D94"/>
+      <selection activeCell="B99" sqref="B99:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,126 +3323,189 @@
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
+      <c r="A95" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="A96" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>460</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>469</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>475</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B87" r:id="rId90" xr:uid="{67E85579-CD16-4DCC-A3F6-C6653F801D89}"/>
-    <hyperlink ref="B93" r:id="rId91" xr:uid="{5EF7A279-F237-497D-B6E1-08B29D7CDC08}"/>
-    <hyperlink ref="B94" r:id="rId92" xr:uid="{B7687CFA-7998-4504-9E18-9B1BA1862F1C}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B20" r:id="rId18"/>
+    <hyperlink ref="B21" r:id="rId19"/>
+    <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B23" r:id="rId21"/>
+    <hyperlink ref="B24" r:id="rId22"/>
+    <hyperlink ref="B25" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
+    <hyperlink ref="B27" r:id="rId25"/>
+    <hyperlink ref="B28" r:id="rId26"/>
+    <hyperlink ref="B29" r:id="rId27"/>
+    <hyperlink ref="B30" r:id="rId28"/>
+    <hyperlink ref="B31" r:id="rId29"/>
+    <hyperlink ref="B32" r:id="rId30"/>
+    <hyperlink ref="B33" r:id="rId31"/>
+    <hyperlink ref="B34" r:id="rId32"/>
+    <hyperlink ref="B35" r:id="rId33"/>
+    <hyperlink ref="B36" r:id="rId34"/>
+    <hyperlink ref="B37" r:id="rId35"/>
+    <hyperlink ref="B38" r:id="rId36"/>
+    <hyperlink ref="B39" r:id="rId37"/>
+    <hyperlink ref="B40" r:id="rId38"/>
+    <hyperlink ref="B41" r:id="rId39"/>
+    <hyperlink ref="B42" r:id="rId40"/>
+    <hyperlink ref="B43" r:id="rId41"/>
+    <hyperlink ref="B44" r:id="rId42"/>
+    <hyperlink ref="B45" r:id="rId43"/>
+    <hyperlink ref="B46" r:id="rId44"/>
+    <hyperlink ref="B47" r:id="rId45"/>
+    <hyperlink ref="B48" r:id="rId46"/>
+    <hyperlink ref="B49" r:id="rId47"/>
+    <hyperlink ref="B50" r:id="rId48"/>
+    <hyperlink ref="B51" r:id="rId49"/>
+    <hyperlink ref="B52" r:id="rId50"/>
+    <hyperlink ref="B53" r:id="rId51"/>
+    <hyperlink ref="B54" r:id="rId52"/>
+    <hyperlink ref="B55" r:id="rId53"/>
+    <hyperlink ref="B56" r:id="rId54"/>
+    <hyperlink ref="B57" r:id="rId55"/>
+    <hyperlink ref="B58" r:id="rId56"/>
+    <hyperlink ref="B59" r:id="rId57"/>
+    <hyperlink ref="B60" r:id="rId58"/>
+    <hyperlink ref="B61" r:id="rId59"/>
+    <hyperlink ref="B62" r:id="rId60"/>
+    <hyperlink ref="B63" r:id="rId61"/>
+    <hyperlink ref="B64" r:id="rId62"/>
+    <hyperlink ref="B65" r:id="rId63"/>
+    <hyperlink ref="B66" r:id="rId64"/>
+    <hyperlink ref="B67" r:id="rId65"/>
+    <hyperlink ref="B68" r:id="rId66"/>
+    <hyperlink ref="B69" r:id="rId67"/>
+    <hyperlink ref="B70" r:id="rId68"/>
+    <hyperlink ref="B71" r:id="rId69"/>
+    <hyperlink ref="B72" r:id="rId70"/>
+    <hyperlink ref="B73" r:id="rId71"/>
+    <hyperlink ref="B74" r:id="rId72"/>
+    <hyperlink ref="B75" r:id="rId73"/>
+    <hyperlink ref="B76" r:id="rId74"/>
+    <hyperlink ref="B77" r:id="rId75"/>
+    <hyperlink ref="B78" r:id="rId76"/>
+    <hyperlink ref="B79" r:id="rId77"/>
+    <hyperlink ref="B80" r:id="rId78"/>
+    <hyperlink ref="B81" r:id="rId79"/>
+    <hyperlink ref="B82" r:id="rId80"/>
+    <hyperlink ref="B83" r:id="rId81"/>
+    <hyperlink ref="B84" r:id="rId82"/>
+    <hyperlink ref="B85" r:id="rId83"/>
+    <hyperlink ref="B86" r:id="rId84"/>
+    <hyperlink ref="B88" r:id="rId85"/>
+    <hyperlink ref="B89" r:id="rId86"/>
+    <hyperlink ref="B90" r:id="rId87"/>
+    <hyperlink ref="B91" r:id="rId88"/>
+    <hyperlink ref="B92" r:id="rId89"/>
+    <hyperlink ref="B87" r:id="rId90"/>
+    <hyperlink ref="B93" r:id="rId91"/>
+    <hyperlink ref="B94" r:id="rId92"/>
+    <hyperlink ref="B95" r:id="rId93"/>
+    <hyperlink ref="B96" r:id="rId94"/>
+    <hyperlink ref="B97" r:id="rId95"/>
+    <hyperlink ref="B98" r:id="rId96"/>
+    <hyperlink ref="B99" r:id="rId97"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId93"/>
+  <pageSetup orientation="portrait" r:id="rId98"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V67" sqref="V67"/>
     </sheetView>
@@ -6086,7 +6262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6164,7 +6340,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7273,11 +7449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AE6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7728,6 +7904,337 @@
         <v>428</v>
       </c>
     </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B8" s="6">
+        <v>500</v>
+      </c>
+      <c r="C8" s="6">
+        <v>4000</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA8" s="9" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="V11" s="6">
+        <v>1000</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>476</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Joint Owner and Beneficiary rest of the scripts
</commit_message>
<xml_diff>
--- a/InstantOpen/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen/src/main/java/com/Resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA58748-0C56-4E76-8812-676CFE5E1CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="516">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1476,12 +1477,114 @@
   </si>
   <si>
     <t>Colt</t>
+  </si>
+  <si>
+    <t>C23946_NonMemberUserCanAddOneJointOwnerAlongWithOneBeneficiary</t>
+  </si>
+  <si>
+    <t>9875768</t>
+  </si>
+  <si>
+    <t>9675755</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>8875686</t>
+  </si>
+  <si>
+    <t>C23947_VerifyTheRequiredFieldsArePopulatedForJointOwnerApplicantForm</t>
+  </si>
+  <si>
+    <t>C23948_VerifyTheRequiredFieldsArePopulatedForBeneficiaryApplicantForm</t>
+  </si>
+  <si>
+    <t>C23963_NonMemberUserCanModifyTheJointOwnerInfo</t>
+  </si>
+  <si>
+    <t>8875688</t>
+  </si>
+  <si>
+    <t>C23964_NonMemberUserCanModifyExistingBeneficiariesInfo</t>
+  </si>
+  <si>
+    <t>8875888</t>
+  </si>
+  <si>
+    <t>C23965_NonMemberUserCanDeleteExistingJointOwner</t>
+  </si>
+  <si>
+    <t>9875766</t>
+  </si>
+  <si>
+    <t>8975888</t>
+  </si>
+  <si>
+    <t>C23966_NonMemberUserCanDeleteExistingBeneficiarydetails</t>
+  </si>
+  <si>
+    <t>8675888</t>
+  </si>
+  <si>
+    <t>C24325_NonMemberUserCanSeeTheAssignedRoleToTheJointOwner</t>
+  </si>
+  <si>
+    <t>8665888</t>
+  </si>
+  <si>
+    <t>C24326_NonMemberUserCanConfirmTheAssignedRoleToTheJointOwner</t>
+  </si>
+  <si>
+    <t>8665898</t>
+  </si>
+  <si>
+    <t>C24327_NonMemberUserCanNotSeeRoleAssignIfNoProductIsSelected</t>
+  </si>
+  <si>
+    <t>8765898</t>
+  </si>
+  <si>
+    <t>8875766</t>
+  </si>
+  <si>
+    <t>C24328_NonMemberUserCanSeeRoleAssignIfClassicCheckingIsSelected</t>
+  </si>
+  <si>
+    <t>8565898</t>
+  </si>
+  <si>
+    <t>C24329_NonMemberUserCanSeeRoleAssignIfHighYieldCheckingIsSelected</t>
+  </si>
+  <si>
+    <t>8566898</t>
+  </si>
+  <si>
+    <t>C24330_NonMemberUserCanSeeTheRoleAssignPageWhileSelectingCreditCard</t>
+  </si>
+  <si>
+    <t>8566878</t>
+  </si>
+  <si>
+    <t>C24331_NonMemberUserCanSeeTheRoleAssignPageWhileSelectingVehicleLoan</t>
+  </si>
+  <si>
+    <t>8566888</t>
+  </si>
+  <si>
+    <t>887557915</t>
+  </si>
+  <si>
+    <t>888557915</t>
+  </si>
+  <si>
+    <t>888556916</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1866,11 +1969,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99:D99"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,118 +3499,328 @@
         <v>7</v>
       </c>
     </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>487</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>489</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>491</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>496</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>498</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>502</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>507</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>511</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
-    <hyperlink ref="B23" r:id="rId21"/>
-    <hyperlink ref="B24" r:id="rId22"/>
-    <hyperlink ref="B25" r:id="rId23"/>
-    <hyperlink ref="B26" r:id="rId24"/>
-    <hyperlink ref="B27" r:id="rId25"/>
-    <hyperlink ref="B28" r:id="rId26"/>
-    <hyperlink ref="B29" r:id="rId27"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B31" r:id="rId29"/>
-    <hyperlink ref="B32" r:id="rId30"/>
-    <hyperlink ref="B33" r:id="rId31"/>
-    <hyperlink ref="B34" r:id="rId32"/>
-    <hyperlink ref="B35" r:id="rId33"/>
-    <hyperlink ref="B36" r:id="rId34"/>
-    <hyperlink ref="B37" r:id="rId35"/>
-    <hyperlink ref="B38" r:id="rId36"/>
-    <hyperlink ref="B39" r:id="rId37"/>
-    <hyperlink ref="B40" r:id="rId38"/>
-    <hyperlink ref="B41" r:id="rId39"/>
-    <hyperlink ref="B42" r:id="rId40"/>
-    <hyperlink ref="B43" r:id="rId41"/>
-    <hyperlink ref="B44" r:id="rId42"/>
-    <hyperlink ref="B45" r:id="rId43"/>
-    <hyperlink ref="B46" r:id="rId44"/>
-    <hyperlink ref="B47" r:id="rId45"/>
-    <hyperlink ref="B48" r:id="rId46"/>
-    <hyperlink ref="B49" r:id="rId47"/>
-    <hyperlink ref="B50" r:id="rId48"/>
-    <hyperlink ref="B51" r:id="rId49"/>
-    <hyperlink ref="B52" r:id="rId50"/>
-    <hyperlink ref="B53" r:id="rId51"/>
-    <hyperlink ref="B54" r:id="rId52"/>
-    <hyperlink ref="B55" r:id="rId53"/>
-    <hyperlink ref="B56" r:id="rId54"/>
-    <hyperlink ref="B57" r:id="rId55"/>
-    <hyperlink ref="B58" r:id="rId56"/>
-    <hyperlink ref="B59" r:id="rId57"/>
-    <hyperlink ref="B60" r:id="rId58"/>
-    <hyperlink ref="B61" r:id="rId59"/>
-    <hyperlink ref="B62" r:id="rId60"/>
-    <hyperlink ref="B63" r:id="rId61"/>
-    <hyperlink ref="B64" r:id="rId62"/>
-    <hyperlink ref="B65" r:id="rId63"/>
-    <hyperlink ref="B66" r:id="rId64"/>
-    <hyperlink ref="B67" r:id="rId65"/>
-    <hyperlink ref="B68" r:id="rId66"/>
-    <hyperlink ref="B69" r:id="rId67"/>
-    <hyperlink ref="B70" r:id="rId68"/>
-    <hyperlink ref="B71" r:id="rId69"/>
-    <hyperlink ref="B72" r:id="rId70"/>
-    <hyperlink ref="B73" r:id="rId71"/>
-    <hyperlink ref="B74" r:id="rId72"/>
-    <hyperlink ref="B75" r:id="rId73"/>
-    <hyperlink ref="B76" r:id="rId74"/>
-    <hyperlink ref="B77" r:id="rId75"/>
-    <hyperlink ref="B78" r:id="rId76"/>
-    <hyperlink ref="B79" r:id="rId77"/>
-    <hyperlink ref="B80" r:id="rId78"/>
-    <hyperlink ref="B81" r:id="rId79"/>
-    <hyperlink ref="B82" r:id="rId80"/>
-    <hyperlink ref="B83" r:id="rId81"/>
-    <hyperlink ref="B84" r:id="rId82"/>
-    <hyperlink ref="B85" r:id="rId83"/>
-    <hyperlink ref="B86" r:id="rId84"/>
-    <hyperlink ref="B88" r:id="rId85"/>
-    <hyperlink ref="B89" r:id="rId86"/>
-    <hyperlink ref="B90" r:id="rId87"/>
-    <hyperlink ref="B91" r:id="rId88"/>
-    <hyperlink ref="B92" r:id="rId89"/>
-    <hyperlink ref="B87" r:id="rId90"/>
-    <hyperlink ref="B93" r:id="rId91"/>
-    <hyperlink ref="B94" r:id="rId92"/>
-    <hyperlink ref="B95" r:id="rId93"/>
-    <hyperlink ref="B96" r:id="rId94"/>
-    <hyperlink ref="B97" r:id="rId95"/>
-    <hyperlink ref="B98" r:id="rId96"/>
-    <hyperlink ref="B99" r:id="rId97"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B87" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B100" r:id="rId98" xr:uid="{4732F8EA-7EAF-4938-BFC3-BB63507C20FF}"/>
+    <hyperlink ref="B101" r:id="rId99" xr:uid="{E19B1B96-6329-4396-B4E6-0869B89EB1A3}"/>
+    <hyperlink ref="B102" r:id="rId100" xr:uid="{38D0988C-2B83-4BE9-9ACC-CD054ED764B5}"/>
+    <hyperlink ref="B103" r:id="rId101" xr:uid="{78E03267-89FE-4A9C-81B2-EB3F8E9BD231}"/>
+    <hyperlink ref="B104" r:id="rId102" xr:uid="{97AE53B7-0109-4917-A2E0-ED48ADBD1B4D}"/>
+    <hyperlink ref="B105" r:id="rId103" xr:uid="{03D2BC44-5E43-45F8-A52C-D111A2F0C9E1}"/>
+    <hyperlink ref="B106" r:id="rId104" xr:uid="{227334BE-F551-4183-91A6-E893E4EFA62F}"/>
+    <hyperlink ref="B107" r:id="rId105" xr:uid="{721F7900-1D35-4402-BFAD-525F8F2A723E}"/>
+    <hyperlink ref="B108" r:id="rId106" xr:uid="{D030F014-E641-4BB7-8782-C8C62736AC69}"/>
+    <hyperlink ref="B109" r:id="rId107" xr:uid="{937F3AE1-DC9B-4755-B144-9A75FD7AD841}"/>
+    <hyperlink ref="B110" r:id="rId108" xr:uid="{D7FCB232-DD09-4129-9046-32DBF4178E43}"/>
+    <hyperlink ref="B111" r:id="rId109" xr:uid="{32D3E926-31A2-4F19-B467-D732DAD2BEE7}"/>
+    <hyperlink ref="B112" r:id="rId110" xr:uid="{7CFB43A0-44E7-4225-9995-5B18450CBB05}"/>
+    <hyperlink ref="B113" r:id="rId111" xr:uid="{5CB72AA3-0C6C-4405-BCAB-1D6A4341298B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId98"/>
+  <pageSetup orientation="portrait" r:id="rId112"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD81"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V67" sqref="V67"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3886,6 +4199,60 @@
       <c r="A14" s="6" t="s">
         <v>92</v>
       </c>
+      <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="X14" s="7" t="s">
         <v>80</v>
       </c>
@@ -3899,6 +4266,60 @@
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>93</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="X15" s="7" t="s">
         <v>80</v>
@@ -3962,8 +4383,62 @@
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>97</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="X19" s="7" t="s">
         <v>80</v>
@@ -6059,7 +6534,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>434</v>
       </c>
@@ -6125,7 +6600,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>438</v>
       </c>
@@ -6189,7 +6664,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>442</v>
       </c>
@@ -6252,6 +6727,901 @@
         <v>85</v>
       </c>
       <c r="Z67" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O68" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P68" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q68" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R68" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S68" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T68" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U68" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="V68" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="W68" s="6"/>
+      <c r="X68" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y68" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z68" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P69" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q69" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R69" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S69" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T69" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U69" s="2"/>
+      <c r="V69" s="2"/>
+      <c r="W69" s="6"/>
+      <c r="X69" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y69" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z69" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA69" s="12"/>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>488</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P70" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q70" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R70" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S70" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T70" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U70" s="2"/>
+      <c r="V70" s="2"/>
+      <c r="W70" s="6"/>
+      <c r="X70" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y70" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z70" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O71" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P71" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q71" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R71" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S71" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T71" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U71" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="V71" s="2"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y71" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z71" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O72" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P72" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q72" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R72" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S72" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T72" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U72" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="V72" s="2"/>
+      <c r="W72" s="6"/>
+      <c r="X72" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y72" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z72" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>493</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O73" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P73" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q73" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R73" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S73" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T73" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U73" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="V73" s="2"/>
+      <c r="W73" s="6"/>
+      <c r="X73" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y73" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z73" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O74" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P74" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q74" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R74" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S74" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U74" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="V74" s="2"/>
+      <c r="W74" s="6"/>
+      <c r="X74" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y74" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z74" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N75" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O75" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P75" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q75" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R75" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S75" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T75" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U75" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="V75" s="2"/>
+      <c r="W75" s="6"/>
+      <c r="X75" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y75" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z75" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>500</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N76" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O76" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P76" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R76" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S76" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T76" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U76" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="V76" s="2"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y76" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z76" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O77" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P77" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R77" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S77" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T77" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U77" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="V77" s="2"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y77" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z77" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>505</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N78" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O78" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P78" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q78" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R78" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S78" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T78" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U78" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="V78" s="2"/>
+      <c r="W78" s="6"/>
+      <c r="X78" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y78" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z78" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N79" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O79" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P79" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q79" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R79" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S79" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T79" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U79" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="V79" s="2"/>
+      <c r="W79" s="6"/>
+      <c r="X79" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y79" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z79" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>509</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N80" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O80" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P80" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q80" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R80" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S80" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T80" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U80" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="V80" s="2"/>
+      <c r="W80" s="6"/>
+      <c r="X80" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y80" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z80" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N81" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O81" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="P81" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q81" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="R81" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S81" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T81" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U81" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="V81" s="2"/>
+      <c r="W81" s="6"/>
+      <c r="X81" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y81" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z81" s="7" t="s">
         <v>82</v>
       </c>
     </row>
@@ -6262,7 +7632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6340,7 +7710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7449,12 +8819,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>